<commit_message>
Several new spreadsheets update
</commit_message>
<xml_diff>
--- a/Option 1/Krause21_Rev03.xlsx
+++ b/Option 1/Krause21_Rev03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Slava\PHYS3116\PHYS3116-Ethan-Slava\Option 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1A336A63-65C2-49B4-BC5C-ECE14F9AA744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{75DDB391-6CCF-43B2-847F-63EB19957010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8EE74A37-30E6-47E8-8656-96CE864E3A87}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EE74A37-30E6-47E8-8656-96CE864E3A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Krause21_Rev03" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="112">
   <si>
     <t>Class</t>
   </si>
@@ -348,6 +348,15 @@
   </si>
   <si>
     <t>Age/FeH</t>
+  </si>
+  <si>
+    <t>Massari 2019</t>
+  </si>
+  <si>
+    <t>Belokurov 2023</t>
+  </si>
+  <si>
+    <t>R_gc</t>
   </si>
 </sst>
 </file>
@@ -490,7 +499,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -682,6 +691,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -843,10 +864,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1222,10 +1252,2322 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D38B78-5540-4D51-A243-EA549ACBF181}">
+  <dimension ref="A1:O62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q53" sqref="Q53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0.39</v>
+      </c>
+      <c r="E2">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F2">
+        <v>0.04</v>
+      </c>
+      <c r="G2">
+        <v>7.4</v>
+      </c>
+      <c r="H2">
+        <v>-0.12</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="M2" s="6">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="E3">
+        <v>3.3</v>
+      </c>
+      <c r="F3">
+        <v>2.92</v>
+      </c>
+      <c r="G3">
+        <v>11.2</v>
+      </c>
+      <c r="H3">
+        <v>-0.44</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3">
+        <v>4.9279999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>2.5</v>
+      </c>
+      <c r="F4">
+        <v>4.8</v>
+      </c>
+      <c r="G4">
+        <v>11.7</v>
+      </c>
+      <c r="H4">
+        <v>-0.45</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4">
+        <v>5.2649999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>2.4E-2</v>
+      </c>
+      <c r="G5">
+        <v>8.6</v>
+      </c>
+      <c r="H5">
+        <v>-0.81</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5">
+        <v>6.9660000000000002</v>
+      </c>
+      <c r="M5" s="6">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>3.38</v>
+      </c>
+      <c r="E6">
+        <v>4.2</v>
+      </c>
+      <c r="F6">
+        <v>0.81</v>
+      </c>
+      <c r="G6">
+        <v>12.7</v>
+      </c>
+      <c r="H6">
+        <v>-0.64</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6">
+        <v>8.1280000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>5.51</v>
+      </c>
+      <c r="E7">
+        <v>3.05</v>
+      </c>
+      <c r="F7">
+        <v>1.81</v>
+      </c>
+      <c r="G7">
+        <v>7.64</v>
+      </c>
+      <c r="H7">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7">
+        <v>8.6332000000000004</v>
+      </c>
+      <c r="M7" s="6">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>5.7</v>
+      </c>
+      <c r="F8">
+        <v>0.35</v>
+      </c>
+      <c r="G8">
+        <v>12.4</v>
+      </c>
+      <c r="H8">
+        <v>-0.7</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>2.57</v>
+      </c>
+      <c r="E9">
+        <v>3.2</v>
+      </c>
+      <c r="F9">
+        <v>0.8</v>
+      </c>
+      <c r="G9">
+        <v>12.5</v>
+      </c>
+      <c r="H9">
+        <v>-0.7</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>0.37</v>
+      </c>
+      <c r="E10">
+        <v>5.68</v>
+      </c>
+      <c r="F10">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G10">
+        <v>12.7</v>
+      </c>
+      <c r="H10">
+        <v>-0.7</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10">
+        <v>8.89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>2.17</v>
+      </c>
+      <c r="E11">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="F11">
+        <v>0.52</v>
+      </c>
+      <c r="G11">
+        <v>13.6</v>
+      </c>
+      <c r="H11">
+        <v>-0.66</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11">
+        <v>8.9760000000000009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>0.3</v>
+      </c>
+      <c r="E12">
+        <v>5.05</v>
+      </c>
+      <c r="F12">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="G12">
+        <v>13.3</v>
+      </c>
+      <c r="H12">
+        <v>-0.73</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12">
+        <v>9.7089999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>6.46</v>
+      </c>
+      <c r="E13">
+        <v>7.1</v>
+      </c>
+      <c r="F13">
+        <v>0.92</v>
+      </c>
+      <c r="G13">
+        <v>12.8</v>
+      </c>
+      <c r="H13">
+        <v>-0.76</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13">
+        <v>9.7279999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>3.66</v>
+      </c>
+      <c r="F14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G14">
+        <v>13.1</v>
+      </c>
+      <c r="H14">
+        <v>-0.78</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14">
+        <v>10.218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>0.2</v>
+      </c>
+      <c r="E15">
+        <v>3.3</v>
+      </c>
+      <c r="F15">
+        <v>0.06</v>
+      </c>
+      <c r="G15">
+        <v>12.7</v>
+      </c>
+      <c r="H15">
+        <v>-0.82</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15">
+        <v>10.414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16">
+        <v>3.41</v>
+      </c>
+      <c r="E16">
+        <v>5.5</v>
+      </c>
+      <c r="F16">
+        <v>0.62</v>
+      </c>
+      <c r="G16">
+        <v>10.24</v>
+      </c>
+      <c r="H16">
+        <v>-1.08</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L16">
+        <v>11.059200000000001</v>
+      </c>
+      <c r="M16" s="6">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E17">
+        <v>2.37</v>
+      </c>
+      <c r="F17">
+        <v>0.46</v>
+      </c>
+      <c r="G17">
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <v>-0.97</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17">
+        <v>11.64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>3.57</v>
+      </c>
+      <c r="E18">
+        <v>6.58</v>
+      </c>
+      <c r="F18">
+        <v>0.54</v>
+      </c>
+      <c r="G18">
+        <v>13.1</v>
+      </c>
+      <c r="H18">
+        <v>-0.96</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18">
+        <v>12.576000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19">
+        <v>2.5</v>
+      </c>
+      <c r="E19">
+        <v>3.5</v>
+      </c>
+      <c r="F19">
+        <v>0.72</v>
+      </c>
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>-1.26</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19">
+        <v>12.6</v>
+      </c>
+      <c r="M19" s="7">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20">
+        <v>1.68</v>
+      </c>
+      <c r="E20">
+        <v>7.82</v>
+      </c>
+      <c r="F20">
+        <v>0.21</v>
+      </c>
+      <c r="G20">
+        <v>10.9</v>
+      </c>
+      <c r="H20">
+        <v>-1.21</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" t="s">
+        <v>36</v>
+      </c>
+      <c r="L20">
+        <v>13.189</v>
+      </c>
+      <c r="M20" s="6">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21">
+        <v>12.3</v>
+      </c>
+      <c r="E21">
+        <v>3.8</v>
+      </c>
+      <c r="F21">
+        <v>3.24</v>
+      </c>
+      <c r="G21">
+        <v>11.2</v>
+      </c>
+      <c r="H21">
+        <v>-1.18</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21">
+        <v>13.215999999999999</v>
+      </c>
+      <c r="M21" s="6">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>0.81</v>
+      </c>
+      <c r="E22">
+        <v>7.7</v>
+      </c>
+      <c r="F22">
+        <v>0.11</v>
+      </c>
+      <c r="G22">
+        <v>13.6</v>
+      </c>
+      <c r="H22">
+        <v>-0.99</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22">
+        <v>13.464</v>
+      </c>
+      <c r="M22" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23">
+        <v>12.9</v>
+      </c>
+      <c r="E23">
+        <v>10.7</v>
+      </c>
+      <c r="F23">
+        <v>1.2</v>
+      </c>
+      <c r="G23">
+        <v>10.8</v>
+      </c>
+      <c r="H23">
+        <v>-1.25</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L23">
+        <v>13.5</v>
+      </c>
+      <c r="M23" s="6">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24">
+        <v>1.17</v>
+      </c>
+      <c r="E24">
+        <v>5.5</v>
+      </c>
+      <c r="F24">
+        <v>0.21</v>
+      </c>
+      <c r="G24">
+        <v>13.4</v>
+      </c>
+      <c r="H24">
+        <v>-1.03</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K24" t="s">
+        <v>43</v>
+      </c>
+      <c r="L24">
+        <v>13.802</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>0.48</v>
+      </c>
+      <c r="E25">
+        <v>2.39</v>
+      </c>
+      <c r="F25">
+        <v>0.2</v>
+      </c>
+      <c r="G25">
+        <v>13.2</v>
+      </c>
+      <c r="H25">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" t="s">
+        <v>45</v>
+      </c>
+      <c r="L25">
+        <v>14.388</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>2.95</v>
+      </c>
+      <c r="E26">
+        <v>5.32</v>
+      </c>
+      <c r="F26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G26">
+        <v>11.1</v>
+      </c>
+      <c r="H26">
+        <v>-1.32</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L26">
+        <v>14.651999999999999</v>
+      </c>
+      <c r="M26" s="6">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>3.03</v>
+      </c>
+      <c r="E27">
+        <v>4.87</v>
+      </c>
+      <c r="F27">
+        <v>0.62</v>
+      </c>
+      <c r="G27">
+        <v>11.3</v>
+      </c>
+      <c r="H27">
+        <v>-1.3</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L27">
+        <v>14.69</v>
+      </c>
+      <c r="M27" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28">
+        <v>4.68</v>
+      </c>
+      <c r="E28">
+        <v>11.7</v>
+      </c>
+      <c r="F28">
+        <v>0.4</v>
+      </c>
+      <c r="G28">
+        <v>11.4</v>
+      </c>
+      <c r="H28">
+        <v>-1.34</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" t="s">
+        <v>48</v>
+      </c>
+      <c r="L28">
+        <v>15.276</v>
+      </c>
+      <c r="M28" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29">
+        <v>3.89</v>
+      </c>
+      <c r="E29">
+        <v>6.6</v>
+      </c>
+      <c r="F29">
+        <v>0.59</v>
+      </c>
+      <c r="G29">
+        <v>11.5</v>
+      </c>
+      <c r="H29">
+        <v>-1.33</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" t="s">
+        <v>50</v>
+      </c>
+      <c r="L29">
+        <v>15.295</v>
+      </c>
+      <c r="M29" s="7">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30">
+        <v>5.75</v>
+      </c>
+      <c r="E30">
+        <v>6.03</v>
+      </c>
+      <c r="F30">
+        <v>0.95</v>
+      </c>
+      <c r="G30">
+        <v>11.8</v>
+      </c>
+      <c r="H30">
+        <v>-1.31</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K30" t="s">
+        <v>52</v>
+      </c>
+      <c r="L30">
+        <v>15.458</v>
+      </c>
+      <c r="M30" s="6">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31">
+        <v>7.75</v>
+      </c>
+      <c r="E31">
+        <v>5.93</v>
+      </c>
+      <c r="F31">
+        <v>1.31</v>
+      </c>
+      <c r="G31">
+        <v>11.7</v>
+      </c>
+      <c r="H31">
+        <v>-1.33</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K31" t="s">
+        <v>54</v>
+      </c>
+      <c r="L31">
+        <v>15.561</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>0.2</v>
+      </c>
+      <c r="E32">
+        <v>2.86</v>
+      </c>
+      <c r="F32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G32">
+        <v>10.5</v>
+      </c>
+      <c r="H32">
+        <v>-1.51</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K32" t="s">
+        <v>56</v>
+      </c>
+      <c r="L32">
+        <v>15.855</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33">
+        <v>0.46</v>
+      </c>
+      <c r="E33">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F33">
+        <v>0.05</v>
+      </c>
+      <c r="G33">
+        <v>12.2</v>
+      </c>
+      <c r="H33">
+        <v>-1.32</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L33">
+        <v>16.103999999999999</v>
+      </c>
+      <c r="M33" s="6">
+        <v>12</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34">
+        <v>5.99</v>
+      </c>
+      <c r="E34">
+        <v>5.04</v>
+      </c>
+      <c r="F34">
+        <v>1.19</v>
+      </c>
+      <c r="G34">
+        <v>12.2</v>
+      </c>
+      <c r="H34">
+        <v>-1.35</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L34">
+        <v>16.47</v>
+      </c>
+      <c r="M34" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E35">
+        <v>7.5</v>
+      </c>
+      <c r="F35">
+        <v>0.15</v>
+      </c>
+      <c r="G35">
+        <v>11.1</v>
+      </c>
+      <c r="H35">
+        <v>-1.51</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L35">
+        <v>16.760999999999999</v>
+      </c>
+      <c r="M35" s="7">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36">
+        <v>1.79</v>
+      </c>
+      <c r="E36">
+        <v>3.16</v>
+      </c>
+      <c r="F36">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G36">
+        <v>12.8</v>
+      </c>
+      <c r="H36">
+        <v>-1.35</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L36">
+        <v>17.28</v>
+      </c>
+      <c r="M36" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <v>7.13</v>
+      </c>
+      <c r="E37">
+        <v>4.2</v>
+      </c>
+      <c r="F37">
+        <v>1.69</v>
+      </c>
+      <c r="G37">
+        <v>12.5</v>
+      </c>
+      <c r="H37">
+        <v>-1.41</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L37">
+        <v>17.625</v>
+      </c>
+      <c r="M37" s="7">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38">
+        <v>0.68</v>
+      </c>
+      <c r="E38">
+        <v>11</v>
+      </c>
+      <c r="F38">
+        <v>0.06</v>
+      </c>
+      <c r="G38">
+        <v>12</v>
+      </c>
+      <c r="H38">
+        <v>-1.5</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K38" t="s">
+        <v>67</v>
+      </c>
+      <c r="L38">
+        <v>18</v>
+      </c>
+      <c r="M38" s="6">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39">
+        <v>3.8</v>
+      </c>
+      <c r="E39">
+        <v>4.2</v>
+      </c>
+      <c r="F39">
+        <v>0.9</v>
+      </c>
+      <c r="G39">
+        <v>11.6</v>
+      </c>
+      <c r="H39">
+        <v>-1.58</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" t="s">
+        <v>68</v>
+      </c>
+      <c r="L39">
+        <v>18.327999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E40">
+        <v>3.02</v>
+      </c>
+      <c r="F40">
+        <v>1.66</v>
+      </c>
+      <c r="G40">
+        <v>12.5</v>
+      </c>
+      <c r="H40">
+        <v>-1.47</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K40" t="s">
+        <v>69</v>
+      </c>
+      <c r="L40">
+        <v>18.375</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41">
+        <v>6.44</v>
+      </c>
+      <c r="E41">
+        <v>5.32</v>
+      </c>
+      <c r="F41">
+        <v>1.21</v>
+      </c>
+      <c r="G41">
+        <v>12.7</v>
+      </c>
+      <c r="H41">
+        <v>-1.49</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K41" t="s">
+        <v>71</v>
+      </c>
+      <c r="L41">
+        <v>18.922999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42">
+        <v>1.45</v>
+      </c>
+      <c r="E42">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F42">
+        <v>0.5</v>
+      </c>
+      <c r="G42">
+        <v>12</v>
+      </c>
+      <c r="H42">
+        <v>-1.58</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K42" t="s">
+        <v>73</v>
+      </c>
+      <c r="L42">
+        <v>18.96</v>
+      </c>
+      <c r="M42" s="6">
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43">
+        <v>0.74</v>
+      </c>
+      <c r="E43">
+        <v>4.2</v>
+      </c>
+      <c r="F43">
+        <v>0.18</v>
+      </c>
+      <c r="G43">
+        <v>13.4</v>
+      </c>
+      <c r="H43">
+        <v>-1.43</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K43" t="s">
+        <v>75</v>
+      </c>
+      <c r="L43">
+        <v>19.161999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44">
+        <v>1.53</v>
+      </c>
+      <c r="E44">
+        <v>4.2</v>
+      </c>
+      <c r="F44">
+        <v>0.36</v>
+      </c>
+      <c r="G44">
+        <v>12.4</v>
+      </c>
+      <c r="H44">
+        <v>-1.57</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K44" t="s">
+        <v>77</v>
+      </c>
+      <c r="L44">
+        <v>19.468</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45">
+        <v>5.72</v>
+      </c>
+      <c r="E45">
+        <v>3.93</v>
+      </c>
+      <c r="F45">
+        <v>1.45</v>
+      </c>
+      <c r="G45">
+        <v>12.9</v>
+      </c>
+      <c r="H45">
+        <v>-1.53</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K45" t="s">
+        <v>79</v>
+      </c>
+      <c r="L45">
+        <v>19.736999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46">
+        <v>2.11</v>
+      </c>
+      <c r="E46">
+        <v>12.7</v>
+      </c>
+      <c r="F46">
+        <v>0.17</v>
+      </c>
+      <c r="G46">
+        <v>12.3</v>
+      </c>
+      <c r="H46">
+        <v>-1.73</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K46" t="s">
+        <v>80</v>
+      </c>
+      <c r="L46">
+        <v>21.279</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E47">
+        <v>7.9</v>
+      </c>
+      <c r="F47">
+        <v>0.52</v>
+      </c>
+      <c r="G47">
+        <v>12.5</v>
+      </c>
+      <c r="H47">
+        <v>-1.71</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L47">
+        <v>21.375</v>
+      </c>
+      <c r="M47" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48">
+        <v>2.82</v>
+      </c>
+      <c r="E48">
+        <v>3.8</v>
+      </c>
+      <c r="F48">
+        <v>0.75</v>
+      </c>
+      <c r="G48">
+        <v>13.8</v>
+      </c>
+      <c r="H48">
+        <v>-1.55</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K48" t="s">
+        <v>83</v>
+      </c>
+      <c r="L48">
+        <v>21.39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49">
+        <v>1.69</v>
+      </c>
+      <c r="E49">
+        <v>7.17</v>
+      </c>
+      <c r="F49">
+        <v>0.24</v>
+      </c>
+      <c r="G49">
+        <v>13.8</v>
+      </c>
+      <c r="H49">
+        <v>-1.56</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L49">
+        <v>21.527999999999999</v>
+      </c>
+      <c r="M49" s="7">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="F50">
+        <v>0.13</v>
+      </c>
+      <c r="G50">
+        <v>12.5</v>
+      </c>
+      <c r="H50">
+        <v>-1.76</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K50" t="s">
+        <v>85</v>
+      </c>
+      <c r="L50">
+        <v>22</v>
+      </c>
+      <c r="M50" s="6">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51">
+        <v>8.26</v>
+      </c>
+      <c r="E51">
+        <v>11.6</v>
+      </c>
+      <c r="F51">
+        <v>0.71</v>
+      </c>
+      <c r="G51">
+        <v>12.7</v>
+      </c>
+      <c r="H51">
+        <v>-1.86</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L51">
+        <v>23.622</v>
+      </c>
+      <c r="M51" s="6">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52">
+        <v>1.25</v>
+      </c>
+      <c r="E52">
+        <v>22.5</v>
+      </c>
+      <c r="F52">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="G52">
+        <v>12.3</v>
+      </c>
+      <c r="H52">
+        <v>-1.98</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L52">
+        <v>24.353999999999999</v>
+      </c>
+      <c r="M52" s="6">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53">
+        <v>0.85</v>
+      </c>
+      <c r="E53">
+        <v>3.1</v>
+      </c>
+      <c r="F53">
+        <v>0.16</v>
+      </c>
+      <c r="G53">
+        <v>12.4</v>
+      </c>
+      <c r="H53">
+        <v>-1.98</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L53">
+        <v>24.552</v>
+      </c>
+      <c r="M53" s="6">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54">
+        <v>1.17</v>
+      </c>
+      <c r="E54">
+        <v>4.7</v>
+      </c>
+      <c r="F54">
+        <v>0.25</v>
+      </c>
+      <c r="G54">
+        <v>13.1</v>
+      </c>
+      <c r="H54">
+        <v>-1.98</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K54" t="s">
+        <v>92</v>
+      </c>
+      <c r="L54">
+        <v>25.937999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" t="s">
+        <v>95</v>
+      </c>
+      <c r="D55">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E55">
+        <v>7.6</v>
+      </c>
+      <c r="F55">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G55">
+        <v>13.8</v>
+      </c>
+      <c r="H55">
+        <v>-1.93</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L55">
+        <v>26.634</v>
+      </c>
+      <c r="M55" s="7">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E56">
+        <v>3.3</v>
+      </c>
+      <c r="F56">
+        <v>0.33</v>
+      </c>
+      <c r="G56">
+        <v>13.4</v>
+      </c>
+      <c r="H56">
+        <v>-1.99</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K56" t="s">
+        <v>96</v>
+      </c>
+      <c r="L56">
+        <v>26.666</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E57">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="F57">
+        <v>0.45</v>
+      </c>
+      <c r="G57">
+        <v>13.7</v>
+      </c>
+      <c r="H57">
+        <v>-2</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L57">
+        <v>27.4</v>
+      </c>
+      <c r="M57" s="7">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" t="s">
+        <v>100</v>
+      </c>
+      <c r="D58">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="E58">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="F58">
+        <v>1.17</v>
+      </c>
+      <c r="G58">
+        <v>13.2</v>
+      </c>
+      <c r="H58">
+        <v>-2.1</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L58">
+        <v>27.72</v>
+      </c>
+      <c r="M58" s="7">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" t="s">
+        <v>102</v>
+      </c>
+      <c r="D59">
+        <v>1.07</v>
+      </c>
+      <c r="E59">
+        <v>7.7</v>
+      </c>
+      <c r="F59">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G59">
+        <v>12.7</v>
+      </c>
+      <c r="H59">
+        <v>-2.27</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L59">
+        <v>28.829000000000001</v>
+      </c>
+      <c r="M59" s="6">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60">
+        <v>1.79</v>
+      </c>
+      <c r="E60">
+        <v>18.2</v>
+      </c>
+      <c r="F60">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="G60">
+        <v>13.6</v>
+      </c>
+      <c r="H60">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L60">
+        <v>29.92</v>
+      </c>
+      <c r="M60" s="6">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" t="s">
+        <v>105</v>
+      </c>
+      <c r="D61">
+        <v>5.13</v>
+      </c>
+      <c r="E61">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>13.6</v>
+      </c>
+      <c r="H61">
+        <v>-2.33</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K61" t="s">
+        <v>104</v>
+      </c>
+      <c r="L61">
+        <v>31.687999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62">
+        <v>1.45</v>
+      </c>
+      <c r="E62">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F62">
+        <v>0.35</v>
+      </c>
+      <c r="G62">
+        <v>14.6</v>
+      </c>
+      <c r="H62">
+        <v>-2.33</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L62">
+        <v>34.018000000000001</v>
+      </c>
+      <c r="M62" s="7">
+        <v>7.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814D8917-F824-44A4-B314-03A402A7C122}">
   <dimension ref="A1:M62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,2022 +3612,6 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>0.39</v>
-      </c>
-      <c r="E2">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="F2">
-        <v>0.04</v>
-      </c>
-      <c r="G2">
-        <v>7.4</v>
-      </c>
-      <c r="H2">
-        <v>-0.12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2">
-        <v>0.88800000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>9.5500000000000007</v>
-      </c>
-      <c r="E3">
-        <v>3.3</v>
-      </c>
-      <c r="F3">
-        <v>2.92</v>
-      </c>
-      <c r="G3">
-        <v>11.2</v>
-      </c>
-      <c r="H3">
-        <v>-0.44</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3">
-        <v>4.9279999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>2.5</v>
-      </c>
-      <c r="F4">
-        <v>4.8</v>
-      </c>
-      <c r="G4">
-        <v>11.7</v>
-      </c>
-      <c r="H4">
-        <v>-0.45</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4">
-        <v>5.2649999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E5">
-        <v>16</v>
-      </c>
-      <c r="F5">
-        <v>2.4E-2</v>
-      </c>
-      <c r="G5">
-        <v>8.6</v>
-      </c>
-      <c r="H5">
-        <v>-0.81</v>
-      </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5">
-        <v>6.9660000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>3.38</v>
-      </c>
-      <c r="E6">
-        <v>4.2</v>
-      </c>
-      <c r="F6">
-        <v>0.81</v>
-      </c>
-      <c r="G6">
-        <v>12.7</v>
-      </c>
-      <c r="H6">
-        <v>-0.64</v>
-      </c>
-      <c r="J6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6">
-        <v>8.1280000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7">
-        <v>5.51</v>
-      </c>
-      <c r="E7">
-        <v>3.05</v>
-      </c>
-      <c r="F7">
-        <v>1.81</v>
-      </c>
-      <c r="G7">
-        <v>7.64</v>
-      </c>
-      <c r="H7">
-        <v>-1.1299999999999999</v>
-      </c>
-      <c r="J7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7">
-        <v>8.6332000000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>5.7</v>
-      </c>
-      <c r="F8">
-        <v>0.35</v>
-      </c>
-      <c r="G8">
-        <v>12.4</v>
-      </c>
-      <c r="H8">
-        <v>-0.7</v>
-      </c>
-      <c r="J8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8">
-        <v>8.68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9">
-        <v>2.57</v>
-      </c>
-      <c r="E9">
-        <v>3.2</v>
-      </c>
-      <c r="F9">
-        <v>0.8</v>
-      </c>
-      <c r="G9">
-        <v>12.5</v>
-      </c>
-      <c r="H9">
-        <v>-0.7</v>
-      </c>
-      <c r="J9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9">
-        <v>8.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10">
-        <v>0.37</v>
-      </c>
-      <c r="E10">
-        <v>5.68</v>
-      </c>
-      <c r="F10">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="G10">
-        <v>12.7</v>
-      </c>
-      <c r="H10">
-        <v>-0.7</v>
-      </c>
-      <c r="J10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10">
-        <v>8.89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>2.17</v>
-      </c>
-      <c r="E11">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="F11">
-        <v>0.52</v>
-      </c>
-      <c r="G11">
-        <v>13.6</v>
-      </c>
-      <c r="H11">
-        <v>-0.66</v>
-      </c>
-      <c r="J11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11">
-        <v>8.9760000000000009</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>0.3</v>
-      </c>
-      <c r="E12">
-        <v>5.05</v>
-      </c>
-      <c r="F12">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="G12">
-        <v>13.3</v>
-      </c>
-      <c r="H12">
-        <v>-0.73</v>
-      </c>
-      <c r="J12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12">
-        <v>9.7089999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13">
-        <v>6.46</v>
-      </c>
-      <c r="E13">
-        <v>7.1</v>
-      </c>
-      <c r="F13">
-        <v>0.92</v>
-      </c>
-      <c r="G13">
-        <v>12.8</v>
-      </c>
-      <c r="H13">
-        <v>-0.76</v>
-      </c>
-      <c r="J13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13">
-        <v>9.7279999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14">
-        <v>3.66</v>
-      </c>
-      <c r="F14">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G14">
-        <v>13.1</v>
-      </c>
-      <c r="H14">
-        <v>-0.78</v>
-      </c>
-      <c r="J14" t="s">
-        <v>26</v>
-      </c>
-      <c r="K14">
-        <v>10.218</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15">
-        <v>0.2</v>
-      </c>
-      <c r="E15">
-        <v>3.3</v>
-      </c>
-      <c r="F15">
-        <v>0.06</v>
-      </c>
-      <c r="G15">
-        <v>12.7</v>
-      </c>
-      <c r="H15">
-        <v>-0.82</v>
-      </c>
-      <c r="J15" t="s">
-        <v>28</v>
-      </c>
-      <c r="K15">
-        <v>10.414</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16">
-        <v>3.41</v>
-      </c>
-      <c r="E16">
-        <v>5.5</v>
-      </c>
-      <c r="F16">
-        <v>0.62</v>
-      </c>
-      <c r="G16">
-        <v>10.24</v>
-      </c>
-      <c r="H16">
-        <v>-1.08</v>
-      </c>
-      <c r="J16" t="s">
-        <v>30</v>
-      </c>
-      <c r="K16">
-        <v>11.059200000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="E17">
-        <v>2.37</v>
-      </c>
-      <c r="F17">
-        <v>0.46</v>
-      </c>
-      <c r="G17">
-        <v>12</v>
-      </c>
-      <c r="H17">
-        <v>-0.97</v>
-      </c>
-      <c r="J17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17">
-        <v>11.64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <v>3.57</v>
-      </c>
-      <c r="E18">
-        <v>6.58</v>
-      </c>
-      <c r="F18">
-        <v>0.54</v>
-      </c>
-      <c r="G18">
-        <v>13.1</v>
-      </c>
-      <c r="H18">
-        <v>-0.96</v>
-      </c>
-      <c r="J18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K18">
-        <v>12.576000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19">
-        <v>2.5</v>
-      </c>
-      <c r="E19">
-        <v>3.5</v>
-      </c>
-      <c r="F19">
-        <v>0.72</v>
-      </c>
-      <c r="G19">
-        <v>10</v>
-      </c>
-      <c r="H19">
-        <v>-1.26</v>
-      </c>
-      <c r="J19" t="s">
-        <v>34</v>
-      </c>
-      <c r="K19">
-        <v>12.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20">
-        <v>1.68</v>
-      </c>
-      <c r="E20">
-        <v>7.82</v>
-      </c>
-      <c r="F20">
-        <v>0.21</v>
-      </c>
-      <c r="G20">
-        <v>10.9</v>
-      </c>
-      <c r="H20">
-        <v>-1.21</v>
-      </c>
-      <c r="J20" t="s">
-        <v>36</v>
-      </c>
-      <c r="K20">
-        <v>13.189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21">
-        <v>12.3</v>
-      </c>
-      <c r="E21">
-        <v>3.8</v>
-      </c>
-      <c r="F21">
-        <v>3.24</v>
-      </c>
-      <c r="G21">
-        <v>11.2</v>
-      </c>
-      <c r="H21">
-        <v>-1.18</v>
-      </c>
-      <c r="J21" t="s">
-        <v>38</v>
-      </c>
-      <c r="K21">
-        <v>13.215999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22">
-        <v>0.81</v>
-      </c>
-      <c r="E22">
-        <v>7.7</v>
-      </c>
-      <c r="F22">
-        <v>0.11</v>
-      </c>
-      <c r="G22">
-        <v>13.6</v>
-      </c>
-      <c r="H22">
-        <v>-0.99</v>
-      </c>
-      <c r="J22" t="s">
-        <v>40</v>
-      </c>
-      <c r="K22">
-        <v>13.464</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23">
-        <v>12.9</v>
-      </c>
-      <c r="E23">
-        <v>10.7</v>
-      </c>
-      <c r="F23">
-        <v>1.2</v>
-      </c>
-      <c r="G23">
-        <v>10.8</v>
-      </c>
-      <c r="H23">
-        <v>-1.25</v>
-      </c>
-      <c r="J23" t="s">
-        <v>41</v>
-      </c>
-      <c r="K23">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24">
-        <v>1.17</v>
-      </c>
-      <c r="E24">
-        <v>5.5</v>
-      </c>
-      <c r="F24">
-        <v>0.21</v>
-      </c>
-      <c r="G24">
-        <v>13.4</v>
-      </c>
-      <c r="H24">
-        <v>-1.03</v>
-      </c>
-      <c r="J24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K24">
-        <v>13.802</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25">
-        <v>0.48</v>
-      </c>
-      <c r="E25">
-        <v>2.39</v>
-      </c>
-      <c r="F25">
-        <v>0.2</v>
-      </c>
-      <c r="G25">
-        <v>13.2</v>
-      </c>
-      <c r="H25">
-        <v>-1.0900000000000001</v>
-      </c>
-      <c r="J25" t="s">
-        <v>45</v>
-      </c>
-      <c r="K25">
-        <v>14.388</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26">
-        <v>2.95</v>
-      </c>
-      <c r="E26">
-        <v>5.32</v>
-      </c>
-      <c r="F26">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G26">
-        <v>11.1</v>
-      </c>
-      <c r="H26">
-        <v>-1.32</v>
-      </c>
-      <c r="J26" t="s">
-        <v>46</v>
-      </c>
-      <c r="K26">
-        <v>14.651999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27">
-        <v>3.03</v>
-      </c>
-      <c r="E27">
-        <v>4.87</v>
-      </c>
-      <c r="F27">
-        <v>0.62</v>
-      </c>
-      <c r="G27">
-        <v>11.3</v>
-      </c>
-      <c r="H27">
-        <v>-1.3</v>
-      </c>
-      <c r="J27" t="s">
-        <v>47</v>
-      </c>
-      <c r="K27">
-        <v>14.69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28">
-        <v>4.68</v>
-      </c>
-      <c r="E28">
-        <v>11.7</v>
-      </c>
-      <c r="F28">
-        <v>0.4</v>
-      </c>
-      <c r="G28">
-        <v>11.4</v>
-      </c>
-      <c r="H28">
-        <v>-1.34</v>
-      </c>
-      <c r="J28" t="s">
-        <v>48</v>
-      </c>
-      <c r="K28">
-        <v>15.276</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29">
-        <v>3.89</v>
-      </c>
-      <c r="E29">
-        <v>6.6</v>
-      </c>
-      <c r="F29">
-        <v>0.59</v>
-      </c>
-      <c r="G29">
-        <v>11.5</v>
-      </c>
-      <c r="H29">
-        <v>-1.33</v>
-      </c>
-      <c r="J29" t="s">
-        <v>50</v>
-      </c>
-      <c r="K29">
-        <v>15.295</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30">
-        <v>5.75</v>
-      </c>
-      <c r="E30">
-        <v>6.03</v>
-      </c>
-      <c r="F30">
-        <v>0.95</v>
-      </c>
-      <c r="G30">
-        <v>11.8</v>
-      </c>
-      <c r="H30">
-        <v>-1.31</v>
-      </c>
-      <c r="J30" t="s">
-        <v>52</v>
-      </c>
-      <c r="K30">
-        <v>15.458</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31">
-        <v>7.75</v>
-      </c>
-      <c r="E31">
-        <v>5.93</v>
-      </c>
-      <c r="F31">
-        <v>1.31</v>
-      </c>
-      <c r="G31">
-        <v>11.7</v>
-      </c>
-      <c r="H31">
-        <v>-1.33</v>
-      </c>
-      <c r="J31" t="s">
-        <v>54</v>
-      </c>
-      <c r="K31">
-        <v>15.561</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32">
-        <v>0.2</v>
-      </c>
-      <c r="E32">
-        <v>2.86</v>
-      </c>
-      <c r="F32">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G32">
-        <v>10.5</v>
-      </c>
-      <c r="H32">
-        <v>-1.51</v>
-      </c>
-      <c r="J32" t="s">
-        <v>56</v>
-      </c>
-      <c r="K32">
-        <v>15.855</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33">
-        <v>0.46</v>
-      </c>
-      <c r="E33">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="F33">
-        <v>0.05</v>
-      </c>
-      <c r="G33">
-        <v>12.2</v>
-      </c>
-      <c r="H33">
-        <v>-1.32</v>
-      </c>
-      <c r="J33" t="s">
-        <v>57</v>
-      </c>
-      <c r="K33">
-        <v>16.103999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34">
-        <v>5.99</v>
-      </c>
-      <c r="E34">
-        <v>5.04</v>
-      </c>
-      <c r="F34">
-        <v>1.19</v>
-      </c>
-      <c r="G34">
-        <v>12.2</v>
-      </c>
-      <c r="H34">
-        <v>-1.35</v>
-      </c>
-      <c r="J34" t="s">
-        <v>59</v>
-      </c>
-      <c r="K34">
-        <v>16.47</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E35">
-        <v>7.5</v>
-      </c>
-      <c r="F35">
-        <v>0.15</v>
-      </c>
-      <c r="G35">
-        <v>11.1</v>
-      </c>
-      <c r="H35">
-        <v>-1.51</v>
-      </c>
-      <c r="J35" t="s">
-        <v>61</v>
-      </c>
-      <c r="K35">
-        <v>16.760999999999999</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36">
-        <v>1.79</v>
-      </c>
-      <c r="E36">
-        <v>3.16</v>
-      </c>
-      <c r="F36">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G36">
-        <v>12.8</v>
-      </c>
-      <c r="H36">
-        <v>-1.35</v>
-      </c>
-      <c r="J36" t="s">
-        <v>64</v>
-      </c>
-      <c r="K36">
-        <v>17.28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37">
-        <v>7.13</v>
-      </c>
-      <c r="E37">
-        <v>4.2</v>
-      </c>
-      <c r="F37">
-        <v>1.69</v>
-      </c>
-      <c r="G37">
-        <v>12.5</v>
-      </c>
-      <c r="H37">
-        <v>-1.41</v>
-      </c>
-      <c r="J37" t="s">
-        <v>66</v>
-      </c>
-      <c r="K37">
-        <v>17.625</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38">
-        <v>0.68</v>
-      </c>
-      <c r="E38">
-        <v>11</v>
-      </c>
-      <c r="F38">
-        <v>0.06</v>
-      </c>
-      <c r="G38">
-        <v>12</v>
-      </c>
-      <c r="H38">
-        <v>-1.5</v>
-      </c>
-      <c r="J38" t="s">
-        <v>67</v>
-      </c>
-      <c r="K38">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39">
-        <v>3.8</v>
-      </c>
-      <c r="E39">
-        <v>4.2</v>
-      </c>
-      <c r="F39">
-        <v>0.9</v>
-      </c>
-      <c r="G39">
-        <v>11.6</v>
-      </c>
-      <c r="H39">
-        <v>-1.58</v>
-      </c>
-      <c r="J39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K39">
-        <v>18.327999999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40">
-        <v>5.0199999999999996</v>
-      </c>
-      <c r="E40">
-        <v>3.02</v>
-      </c>
-      <c r="F40">
-        <v>1.66</v>
-      </c>
-      <c r="G40">
-        <v>12.5</v>
-      </c>
-      <c r="H40">
-        <v>-1.47</v>
-      </c>
-      <c r="J40" t="s">
-        <v>69</v>
-      </c>
-      <c r="K40">
-        <v>18.375</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41">
-        <v>6.44</v>
-      </c>
-      <c r="E41">
-        <v>5.32</v>
-      </c>
-      <c r="F41">
-        <v>1.21</v>
-      </c>
-      <c r="G41">
-        <v>12.7</v>
-      </c>
-      <c r="H41">
-        <v>-1.49</v>
-      </c>
-      <c r="J41" t="s">
-        <v>71</v>
-      </c>
-      <c r="K41">
-        <v>18.922999999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42">
-        <v>1.45</v>
-      </c>
-      <c r="E42">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F42">
-        <v>0.5</v>
-      </c>
-      <c r="G42">
-        <v>12</v>
-      </c>
-      <c r="H42">
-        <v>-1.58</v>
-      </c>
-      <c r="J42" t="s">
-        <v>73</v>
-      </c>
-      <c r="K42">
-        <v>18.96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43">
-        <v>0.74</v>
-      </c>
-      <c r="E43">
-        <v>4.2</v>
-      </c>
-      <c r="F43">
-        <v>0.18</v>
-      </c>
-      <c r="G43">
-        <v>13.4</v>
-      </c>
-      <c r="H43">
-        <v>-1.43</v>
-      </c>
-      <c r="J43" t="s">
-        <v>75</v>
-      </c>
-      <c r="K43">
-        <v>19.161999999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" t="s">
-        <v>77</v>
-      </c>
-      <c r="C44" t="s">
-        <v>78</v>
-      </c>
-      <c r="D44">
-        <v>1.53</v>
-      </c>
-      <c r="E44">
-        <v>4.2</v>
-      </c>
-      <c r="F44">
-        <v>0.36</v>
-      </c>
-      <c r="G44">
-        <v>12.4</v>
-      </c>
-      <c r="H44">
-        <v>-1.57</v>
-      </c>
-      <c r="J44" t="s">
-        <v>77</v>
-      </c>
-      <c r="K44">
-        <v>19.468</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45">
-        <v>5.72</v>
-      </c>
-      <c r="E45">
-        <v>3.93</v>
-      </c>
-      <c r="F45">
-        <v>1.45</v>
-      </c>
-      <c r="G45">
-        <v>12.9</v>
-      </c>
-      <c r="H45">
-        <v>-1.53</v>
-      </c>
-      <c r="J45" t="s">
-        <v>79</v>
-      </c>
-      <c r="K45">
-        <v>19.736999999999998</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46">
-        <v>2.11</v>
-      </c>
-      <c r="E46">
-        <v>12.7</v>
-      </c>
-      <c r="F46">
-        <v>0.17</v>
-      </c>
-      <c r="G46">
-        <v>12.3</v>
-      </c>
-      <c r="H46">
-        <v>-1.73</v>
-      </c>
-      <c r="J46" t="s">
-        <v>80</v>
-      </c>
-      <c r="K46">
-        <v>21.279</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" t="s">
-        <v>82</v>
-      </c>
-      <c r="D47">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E47">
-        <v>7.9</v>
-      </c>
-      <c r="F47">
-        <v>0.52</v>
-      </c>
-      <c r="G47">
-        <v>12.5</v>
-      </c>
-      <c r="H47">
-        <v>-1.71</v>
-      </c>
-      <c r="J47" t="s">
-        <v>81</v>
-      </c>
-      <c r="K47">
-        <v>21.375</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>10</v>
-      </c>
-      <c r="B48" t="s">
-        <v>83</v>
-      </c>
-      <c r="C48" t="s">
-        <v>12</v>
-      </c>
-      <c r="D48">
-        <v>2.82</v>
-      </c>
-      <c r="E48">
-        <v>3.8</v>
-      </c>
-      <c r="F48">
-        <v>0.75</v>
-      </c>
-      <c r="G48">
-        <v>13.8</v>
-      </c>
-      <c r="H48">
-        <v>-1.55</v>
-      </c>
-      <c r="J48" t="s">
-        <v>83</v>
-      </c>
-      <c r="K48">
-        <v>21.39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>10</v>
-      </c>
-      <c r="B49" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" t="s">
-        <v>12</v>
-      </c>
-      <c r="D49">
-        <v>1.69</v>
-      </c>
-      <c r="E49">
-        <v>7.17</v>
-      </c>
-      <c r="F49">
-        <v>0.24</v>
-      </c>
-      <c r="G49">
-        <v>13.8</v>
-      </c>
-      <c r="H49">
-        <v>-1.56</v>
-      </c>
-      <c r="J49" t="s">
-        <v>84</v>
-      </c>
-      <c r="K49">
-        <v>21.527999999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>8</v>
-      </c>
-      <c r="F50">
-        <v>0.13</v>
-      </c>
-      <c r="G50">
-        <v>12.5</v>
-      </c>
-      <c r="H50">
-        <v>-1.76</v>
-      </c>
-      <c r="J50" t="s">
-        <v>85</v>
-      </c>
-      <c r="K50">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>10</v>
-      </c>
-      <c r="B51" t="s">
-        <v>87</v>
-      </c>
-      <c r="C51" t="s">
-        <v>88</v>
-      </c>
-      <c r="D51">
-        <v>8.26</v>
-      </c>
-      <c r="E51">
-        <v>11.6</v>
-      </c>
-      <c r="F51">
-        <v>0.71</v>
-      </c>
-      <c r="G51">
-        <v>12.7</v>
-      </c>
-      <c r="H51">
-        <v>-1.86</v>
-      </c>
-      <c r="J51" t="s">
-        <v>87</v>
-      </c>
-      <c r="K51">
-        <v>23.622</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>10</v>
-      </c>
-      <c r="B52" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52">
-        <v>1.25</v>
-      </c>
-      <c r="E52">
-        <v>22.5</v>
-      </c>
-      <c r="F52">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="G52">
-        <v>12.3</v>
-      </c>
-      <c r="H52">
-        <v>-1.98</v>
-      </c>
-      <c r="J52" t="s">
-        <v>89</v>
-      </c>
-      <c r="K52">
-        <v>24.353999999999999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>10</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D53">
-        <v>0.85</v>
-      </c>
-      <c r="E53">
-        <v>3.1</v>
-      </c>
-      <c r="F53">
-        <v>0.16</v>
-      </c>
-      <c r="G53">
-        <v>12.4</v>
-      </c>
-      <c r="H53">
-        <v>-1.98</v>
-      </c>
-      <c r="J53" t="s">
-        <v>90</v>
-      </c>
-      <c r="K53">
-        <v>24.552</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" t="s">
-        <v>93</v>
-      </c>
-      <c r="D54">
-        <v>1.17</v>
-      </c>
-      <c r="E54">
-        <v>4.7</v>
-      </c>
-      <c r="F54">
-        <v>0.25</v>
-      </c>
-      <c r="G54">
-        <v>13.1</v>
-      </c>
-      <c r="H54">
-        <v>-1.98</v>
-      </c>
-      <c r="J54" t="s">
-        <v>92</v>
-      </c>
-      <c r="K54">
-        <v>25.937999999999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>10</v>
-      </c>
-      <c r="B55" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" t="s">
-        <v>95</v>
-      </c>
-      <c r="D55">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E55">
-        <v>7.6</v>
-      </c>
-      <c r="F55">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G55">
-        <v>13.8</v>
-      </c>
-      <c r="H55">
-        <v>-1.93</v>
-      </c>
-      <c r="J55" t="s">
-        <v>94</v>
-      </c>
-      <c r="K55">
-        <v>26.634</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" t="s">
-        <v>96</v>
-      </c>
-      <c r="C56" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E56">
-        <v>3.3</v>
-      </c>
-      <c r="F56">
-        <v>0.33</v>
-      </c>
-      <c r="G56">
-        <v>13.4</v>
-      </c>
-      <c r="H56">
-        <v>-1.99</v>
-      </c>
-      <c r="J56" t="s">
-        <v>96</v>
-      </c>
-      <c r="K56">
-        <v>26.666</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>10</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D57">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E57">
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="F57">
-        <v>0.45</v>
-      </c>
-      <c r="G57">
-        <v>13.7</v>
-      </c>
-      <c r="H57">
-        <v>-2</v>
-      </c>
-      <c r="J57" t="s">
-        <v>97</v>
-      </c>
-      <c r="K57">
-        <v>27.4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>10</v>
-      </c>
-      <c r="B58" t="s">
-        <v>99</v>
-      </c>
-      <c r="C58" t="s">
-        <v>100</v>
-      </c>
-      <c r="D58">
-        <v>4.8899999999999997</v>
-      </c>
-      <c r="E58">
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="F58">
-        <v>1.17</v>
-      </c>
-      <c r="G58">
-        <v>13.2</v>
-      </c>
-      <c r="H58">
-        <v>-2.1</v>
-      </c>
-      <c r="J58" t="s">
-        <v>99</v>
-      </c>
-      <c r="K58">
-        <v>27.72</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>10</v>
-      </c>
-      <c r="B59" t="s">
-        <v>101</v>
-      </c>
-      <c r="C59" t="s">
-        <v>102</v>
-      </c>
-      <c r="D59">
-        <v>1.07</v>
-      </c>
-      <c r="E59">
-        <v>7.7</v>
-      </c>
-      <c r="F59">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G59">
-        <v>12.7</v>
-      </c>
-      <c r="H59">
-        <v>-2.27</v>
-      </c>
-      <c r="J59" t="s">
-        <v>101</v>
-      </c>
-      <c r="K59">
-        <v>28.829000000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>10</v>
-      </c>
-      <c r="B60" t="s">
-        <v>103</v>
-      </c>
-      <c r="C60" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60">
-        <v>1.79</v>
-      </c>
-      <c r="E60">
-        <v>18.2</v>
-      </c>
-      <c r="F60">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="G60">
-        <v>13.6</v>
-      </c>
-      <c r="H60">
-        <v>-2.2000000000000002</v>
-      </c>
-      <c r="J60" t="s">
-        <v>103</v>
-      </c>
-      <c r="K60">
-        <v>29.92</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>10</v>
-      </c>
-      <c r="B61" t="s">
-        <v>104</v>
-      </c>
-      <c r="C61" t="s">
-        <v>105</v>
-      </c>
-      <c r="D61">
-        <v>5.13</v>
-      </c>
-      <c r="E61">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="F61">
-        <v>1</v>
-      </c>
-      <c r="G61">
-        <v>13.6</v>
-      </c>
-      <c r="H61">
-        <v>-2.33</v>
-      </c>
-      <c r="J61" t="s">
-        <v>104</v>
-      </c>
-      <c r="K61">
-        <v>31.687999999999999</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>10</v>
-      </c>
-      <c r="B62" t="s">
-        <v>106</v>
-      </c>
-      <c r="C62" t="s">
-        <v>107</v>
-      </c>
-      <c r="D62">
-        <v>1.45</v>
-      </c>
-      <c r="E62">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F62">
-        <v>0.35</v>
-      </c>
-      <c r="G62">
-        <v>14.6</v>
-      </c>
-      <c r="H62">
-        <v>-2.33</v>
-      </c>
-      <c r="J62" t="s">
-        <v>106</v>
-      </c>
-      <c r="K62">
-        <v>34.018000000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814D8917-F824-44A4-B314-03A402A7C122}">
-  <dimension ref="A1:M62"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4553,10 +4879,10 @@
       <c r="A40" t="s">
         <v>10</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D40">
@@ -4883,7 +5209,7 @@
       <c r="A50" t="s">
         <v>10</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C50" t="s">

</xml_diff>

<commit_message>
Attempt to use spatial distribution of the in-situ and accreted MW GCs classified as per method described in Belokurov & Kravtsov 2023
</commit_message>
<xml_diff>
--- a/Option 1/Krause21_Rev03.xlsx
+++ b/Option 1/Krause21_Rev03.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Slava\PHYS3116\PHYS3116-Ethan-Slava\Option 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{75DDB391-6CCF-43B2-847F-63EB19957010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3059C05F-1AD2-442B-A738-74BBF013825A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EE74A37-30E6-47E8-8656-96CE864E3A87}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8EE74A37-30E6-47E8-8656-96CE864E3A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Krause21_Rev03" sheetId="1" r:id="rId1"/>
     <sheet name="Krause21_Rev03b" sheetId="2" r:id="rId2"/>
+    <sheet name="Krause21_Rev03c" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="112">
   <si>
     <t>Class</t>
   </si>
@@ -1254,7 +1255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D38B78-5540-4D51-A243-EA549ACBF181}">
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q53" sqref="Q53"/>
     </sheetView>
   </sheetViews>
@@ -5640,4 +5641,2319 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5A9D1F-4AC9-4BE5-88AA-D6F99F935C36}">
+  <dimension ref="A1:O62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>6.46</v>
+      </c>
+      <c r="E2">
+        <v>7.1</v>
+      </c>
+      <c r="F2">
+        <v>0.92</v>
+      </c>
+      <c r="G2">
+        <v>12.8</v>
+      </c>
+      <c r="H2">
+        <v>-0.76</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2">
+        <v>9.7279999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3">
+        <v>0.46</v>
+      </c>
+      <c r="E3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F3">
+        <v>0.05</v>
+      </c>
+      <c r="G3">
+        <v>12.2</v>
+      </c>
+      <c r="H3">
+        <v>-1.32</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3">
+        <v>16.103999999999999</v>
+      </c>
+      <c r="M3" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>2.5</v>
+      </c>
+      <c r="E4">
+        <v>3.5</v>
+      </c>
+      <c r="F4">
+        <v>0.72</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>-1.26</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4">
+        <v>12.6</v>
+      </c>
+      <c r="M4" s="7">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>3.41</v>
+      </c>
+      <c r="E5">
+        <v>5.5</v>
+      </c>
+      <c r="F5">
+        <v>0.62</v>
+      </c>
+      <c r="G5">
+        <v>10.24</v>
+      </c>
+      <c r="H5">
+        <v>-1.08</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5">
+        <v>11.059200000000001</v>
+      </c>
+      <c r="M5" s="6">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>5.51</v>
+      </c>
+      <c r="E6">
+        <v>3.05</v>
+      </c>
+      <c r="F6">
+        <v>1.81</v>
+      </c>
+      <c r="G6">
+        <v>7.64</v>
+      </c>
+      <c r="H6">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6">
+        <v>8.6332000000000004</v>
+      </c>
+      <c r="M6" s="6">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7">
+        <v>1.45</v>
+      </c>
+      <c r="E7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>-1.58</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7">
+        <v>18.96</v>
+      </c>
+      <c r="M7" s="6">
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8">
+        <v>0.85</v>
+      </c>
+      <c r="E8">
+        <v>3.1</v>
+      </c>
+      <c r="F8">
+        <v>0.16</v>
+      </c>
+      <c r="G8">
+        <v>12.4</v>
+      </c>
+      <c r="H8">
+        <v>-1.98</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8">
+        <v>24.552</v>
+      </c>
+      <c r="M8" s="6">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9">
+        <v>12.3</v>
+      </c>
+      <c r="E9">
+        <v>3.8</v>
+      </c>
+      <c r="F9">
+        <v>3.24</v>
+      </c>
+      <c r="G9">
+        <v>11.2</v>
+      </c>
+      <c r="H9">
+        <v>-1.18</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9">
+        <v>13.215999999999999</v>
+      </c>
+      <c r="M9" s="6">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E10">
+        <v>7.5</v>
+      </c>
+      <c r="F10">
+        <v>0.15</v>
+      </c>
+      <c r="G10">
+        <v>11.1</v>
+      </c>
+      <c r="H10">
+        <v>-1.51</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10">
+        <v>16.760999999999999</v>
+      </c>
+      <c r="M10" s="7">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11">
+        <v>1.07</v>
+      </c>
+      <c r="E11">
+        <v>7.7</v>
+      </c>
+      <c r="F11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G11">
+        <v>12.7</v>
+      </c>
+      <c r="H11">
+        <v>-2.27</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L11">
+        <v>28.829000000000001</v>
+      </c>
+      <c r="M11" s="6">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E12">
+        <v>7.9</v>
+      </c>
+      <c r="F12">
+        <v>0.52</v>
+      </c>
+      <c r="G12">
+        <v>12.5</v>
+      </c>
+      <c r="H12">
+        <v>-1.71</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L12">
+        <v>21.375</v>
+      </c>
+      <c r="M12" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13">
+        <v>8.26</v>
+      </c>
+      <c r="E13">
+        <v>11.6</v>
+      </c>
+      <c r="F13">
+        <v>0.71</v>
+      </c>
+      <c r="G13">
+        <v>12.7</v>
+      </c>
+      <c r="H13">
+        <v>-1.86</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L13">
+        <v>23.622</v>
+      </c>
+      <c r="M13" s="6">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>1.25</v>
+      </c>
+      <c r="E14">
+        <v>22.5</v>
+      </c>
+      <c r="F14">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="G14">
+        <v>12.3</v>
+      </c>
+      <c r="H14">
+        <v>-1.98</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L14">
+        <v>24.353999999999999</v>
+      </c>
+      <c r="M14" s="6">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15">
+        <v>4.68</v>
+      </c>
+      <c r="E15">
+        <v>11.7</v>
+      </c>
+      <c r="F15">
+        <v>0.4</v>
+      </c>
+      <c r="G15">
+        <v>11.4</v>
+      </c>
+      <c r="H15">
+        <v>-1.34</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15">
+        <v>15.276</v>
+      </c>
+      <c r="M15" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>7.13</v>
+      </c>
+      <c r="E16">
+        <v>4.2</v>
+      </c>
+      <c r="F16">
+        <v>1.69</v>
+      </c>
+      <c r="G16">
+        <v>12.5</v>
+      </c>
+      <c r="H16">
+        <v>-1.41</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16">
+        <v>17.625</v>
+      </c>
+      <c r="M16" s="7">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>1.79</v>
+      </c>
+      <c r="E17">
+        <v>18.2</v>
+      </c>
+      <c r="F17">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="G17">
+        <v>13.6</v>
+      </c>
+      <c r="H17">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L17">
+        <v>29.92</v>
+      </c>
+      <c r="M17" s="6">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>2.11</v>
+      </c>
+      <c r="E18">
+        <v>12.7</v>
+      </c>
+      <c r="F18">
+        <v>0.17</v>
+      </c>
+      <c r="G18">
+        <v>12.3</v>
+      </c>
+      <c r="H18">
+        <v>-1.73</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K18" t="s">
+        <v>80</v>
+      </c>
+      <c r="L18">
+        <v>21.279</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19">
+        <v>3.89</v>
+      </c>
+      <c r="E19">
+        <v>6.6</v>
+      </c>
+      <c r="F19">
+        <v>0.59</v>
+      </c>
+      <c r="G19">
+        <v>11.5</v>
+      </c>
+      <c r="H19">
+        <v>-1.33</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19">
+        <v>15.295</v>
+      </c>
+      <c r="M19" s="7">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>3.38</v>
+      </c>
+      <c r="E20">
+        <v>4.2</v>
+      </c>
+      <c r="F20">
+        <v>0.81</v>
+      </c>
+      <c r="G20">
+        <v>12.7</v>
+      </c>
+      <c r="H20">
+        <v>-0.64</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20">
+        <v>8.1280000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>5.99</v>
+      </c>
+      <c r="E21">
+        <v>5.04</v>
+      </c>
+      <c r="F21">
+        <v>1.19</v>
+      </c>
+      <c r="G21">
+        <v>12.2</v>
+      </c>
+      <c r="H21">
+        <v>-1.35</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L21">
+        <v>16.47</v>
+      </c>
+      <c r="M21" s="7">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E22">
+        <v>3.02</v>
+      </c>
+      <c r="F22">
+        <v>1.66</v>
+      </c>
+      <c r="G22">
+        <v>12.5</v>
+      </c>
+      <c r="H22">
+        <v>-1.47</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22">
+        <v>18.375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>0.13</v>
+      </c>
+      <c r="G23">
+        <v>12.5</v>
+      </c>
+      <c r="H23">
+        <v>-1.76</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K23" t="s">
+        <v>85</v>
+      </c>
+      <c r="L23">
+        <v>22</v>
+      </c>
+      <c r="M23" s="6">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24">
+        <v>1.17</v>
+      </c>
+      <c r="E24">
+        <v>4.7</v>
+      </c>
+      <c r="F24">
+        <v>0.25</v>
+      </c>
+      <c r="G24">
+        <v>13.1</v>
+      </c>
+      <c r="H24">
+        <v>-1.98</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K24" t="s">
+        <v>92</v>
+      </c>
+      <c r="L24">
+        <v>25.937999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>3.8</v>
+      </c>
+      <c r="E25">
+        <v>4.2</v>
+      </c>
+      <c r="F25">
+        <v>0.9</v>
+      </c>
+      <c r="G25">
+        <v>11.6</v>
+      </c>
+      <c r="H25">
+        <v>-1.58</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K25" t="s">
+        <v>68</v>
+      </c>
+      <c r="L25">
+        <v>18.327999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>1.69</v>
+      </c>
+      <c r="E26">
+        <v>7.17</v>
+      </c>
+      <c r="F26">
+        <v>0.24</v>
+      </c>
+      <c r="G26">
+        <v>13.8</v>
+      </c>
+      <c r="H26">
+        <v>-1.56</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L26">
+        <v>21.527999999999999</v>
+      </c>
+      <c r="M26" s="7">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27">
+        <v>1.17</v>
+      </c>
+      <c r="E27">
+        <v>5.5</v>
+      </c>
+      <c r="F27">
+        <v>0.21</v>
+      </c>
+      <c r="G27">
+        <v>13.4</v>
+      </c>
+      <c r="H27">
+        <v>-1.03</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K27" t="s">
+        <v>43</v>
+      </c>
+      <c r="L27">
+        <v>13.802</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28">
+        <v>7.75</v>
+      </c>
+      <c r="E28">
+        <v>5.93</v>
+      </c>
+      <c r="F28">
+        <v>1.31</v>
+      </c>
+      <c r="G28">
+        <v>11.7</v>
+      </c>
+      <c r="H28">
+        <v>-1.33</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K28" t="s">
+        <v>54</v>
+      </c>
+      <c r="L28">
+        <v>15.561</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29">
+        <v>0.74</v>
+      </c>
+      <c r="E29">
+        <v>4.2</v>
+      </c>
+      <c r="F29">
+        <v>0.18</v>
+      </c>
+      <c r="G29">
+        <v>13.4</v>
+      </c>
+      <c r="H29">
+        <v>-1.43</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K29" t="s">
+        <v>75</v>
+      </c>
+      <c r="L29">
+        <v>19.161999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30">
+        <v>1.53</v>
+      </c>
+      <c r="E30">
+        <v>4.2</v>
+      </c>
+      <c r="F30">
+        <v>0.36</v>
+      </c>
+      <c r="G30">
+        <v>12.4</v>
+      </c>
+      <c r="H30">
+        <v>-1.57</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K30" t="s">
+        <v>77</v>
+      </c>
+      <c r="L30">
+        <v>19.468</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31">
+        <v>2.17</v>
+      </c>
+      <c r="E31">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="F31">
+        <v>0.52</v>
+      </c>
+      <c r="G31">
+        <v>13.6</v>
+      </c>
+      <c r="H31">
+        <v>-0.66</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31">
+        <v>8.9760000000000009</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="E32">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="F32">
+        <v>1.17</v>
+      </c>
+      <c r="G32">
+        <v>13.2</v>
+      </c>
+      <c r="H32">
+        <v>-2.1</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L32">
+        <v>27.72</v>
+      </c>
+      <c r="M32" s="7">
+        <v>9.6</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33">
+        <v>0.37</v>
+      </c>
+      <c r="E33">
+        <v>5.68</v>
+      </c>
+      <c r="F33">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G33">
+        <v>12.7</v>
+      </c>
+      <c r="H33">
+        <v>-0.7</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33">
+        <v>8.89</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34">
+        <v>0.81</v>
+      </c>
+      <c r="E34">
+        <v>7.7</v>
+      </c>
+      <c r="F34">
+        <v>0.11</v>
+      </c>
+      <c r="G34">
+        <v>13.6</v>
+      </c>
+      <c r="H34">
+        <v>-0.99</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L34">
+        <v>13.464</v>
+      </c>
+      <c r="M34" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35">
+        <v>0.3</v>
+      </c>
+      <c r="E35">
+        <v>5.05</v>
+      </c>
+      <c r="F35">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="G35">
+        <v>13.3</v>
+      </c>
+      <c r="H35">
+        <v>-0.73</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" t="s">
+        <v>23</v>
+      </c>
+      <c r="L35">
+        <v>9.7089999999999996</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36">
+        <v>12</v>
+      </c>
+      <c r="E36">
+        <v>2.5</v>
+      </c>
+      <c r="F36">
+        <v>4.8</v>
+      </c>
+      <c r="G36">
+        <v>11.7</v>
+      </c>
+      <c r="H36">
+        <v>-0.45</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" t="s">
+        <v>14</v>
+      </c>
+      <c r="L36">
+        <v>5.2649999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E37">
+        <v>3.3</v>
+      </c>
+      <c r="F37">
+        <v>0.33</v>
+      </c>
+      <c r="G37">
+        <v>13.4</v>
+      </c>
+      <c r="H37">
+        <v>-1.99</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K37" t="s">
+        <v>96</v>
+      </c>
+      <c r="L37">
+        <v>26.666</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="E38">
+        <v>3.3</v>
+      </c>
+      <c r="F38">
+        <v>2.92</v>
+      </c>
+      <c r="G38">
+        <v>11.2</v>
+      </c>
+      <c r="H38">
+        <v>-0.44</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" t="s">
+        <v>13</v>
+      </c>
+      <c r="L38">
+        <v>4.9279999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>5.7</v>
+      </c>
+      <c r="F39">
+        <v>0.35</v>
+      </c>
+      <c r="G39">
+        <v>12.4</v>
+      </c>
+      <c r="H39">
+        <v>-0.7</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" t="s">
+        <v>19</v>
+      </c>
+      <c r="L39">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40">
+        <v>0.2</v>
+      </c>
+      <c r="E40">
+        <v>2.86</v>
+      </c>
+      <c r="F40">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G40">
+        <v>10.5</v>
+      </c>
+      <c r="H40">
+        <v>-1.51</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K40" t="s">
+        <v>56</v>
+      </c>
+      <c r="L40">
+        <v>15.855</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41">
+        <v>5.72</v>
+      </c>
+      <c r="E41">
+        <v>3.93</v>
+      </c>
+      <c r="F41">
+        <v>1.45</v>
+      </c>
+      <c r="G41">
+        <v>12.9</v>
+      </c>
+      <c r="H41">
+        <v>-1.53</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K41" t="s">
+        <v>79</v>
+      </c>
+      <c r="L41">
+        <v>19.736999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42">
+        <v>3.03</v>
+      </c>
+      <c r="E42">
+        <v>4.87</v>
+      </c>
+      <c r="F42">
+        <v>0.62</v>
+      </c>
+      <c r="G42">
+        <v>11.3</v>
+      </c>
+      <c r="H42">
+        <v>-1.3</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L42">
+        <v>14.69</v>
+      </c>
+      <c r="M42" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43">
+        <v>2.57</v>
+      </c>
+      <c r="E43">
+        <v>3.2</v>
+      </c>
+      <c r="F43">
+        <v>0.8</v>
+      </c>
+      <c r="G43">
+        <v>12.5</v>
+      </c>
+      <c r="H43">
+        <v>-0.7</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K43" t="s">
+        <v>20</v>
+      </c>
+      <c r="L43">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>3.66</v>
+      </c>
+      <c r="F44">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G44">
+        <v>13.1</v>
+      </c>
+      <c r="H44">
+        <v>-0.78</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K44" t="s">
+        <v>26</v>
+      </c>
+      <c r="L44">
+        <v>10.218</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E45">
+        <v>2.37</v>
+      </c>
+      <c r="F45">
+        <v>0.46</v>
+      </c>
+      <c r="G45">
+        <v>12</v>
+      </c>
+      <c r="H45">
+        <v>-0.97</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K45" t="s">
+        <v>32</v>
+      </c>
+      <c r="L45">
+        <v>11.64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46">
+        <v>6.44</v>
+      </c>
+      <c r="E46">
+        <v>5.32</v>
+      </c>
+      <c r="F46">
+        <v>1.21</v>
+      </c>
+      <c r="G46">
+        <v>12.7</v>
+      </c>
+      <c r="H46">
+        <v>-1.49</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K46" t="s">
+        <v>71</v>
+      </c>
+      <c r="L46">
+        <v>18.922999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47">
+        <v>1.79</v>
+      </c>
+      <c r="E47">
+        <v>3.16</v>
+      </c>
+      <c r="F47">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G47">
+        <v>12.8</v>
+      </c>
+      <c r="H47">
+        <v>-1.35</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L47">
+        <v>17.28</v>
+      </c>
+      <c r="M47" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48">
+        <v>12.9</v>
+      </c>
+      <c r="E48">
+        <v>10.7</v>
+      </c>
+      <c r="F48">
+        <v>1.2</v>
+      </c>
+      <c r="G48">
+        <v>10.8</v>
+      </c>
+      <c r="H48">
+        <v>-1.25</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L48">
+        <v>13.5</v>
+      </c>
+      <c r="M48" s="6">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49">
+        <v>0.48</v>
+      </c>
+      <c r="E49">
+        <v>2.39</v>
+      </c>
+      <c r="F49">
+        <v>0.2</v>
+      </c>
+      <c r="G49">
+        <v>13.2</v>
+      </c>
+      <c r="H49">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K49" t="s">
+        <v>45</v>
+      </c>
+      <c r="L49">
+        <v>14.388</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50">
+        <v>3.57</v>
+      </c>
+      <c r="E50">
+        <v>6.58</v>
+      </c>
+      <c r="F50">
+        <v>0.54</v>
+      </c>
+      <c r="G50">
+        <v>13.1</v>
+      </c>
+      <c r="H50">
+        <v>-0.96</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K50" t="s">
+        <v>33</v>
+      </c>
+      <c r="L50">
+        <v>12.576000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51">
+        <v>2.82</v>
+      </c>
+      <c r="E51">
+        <v>3.8</v>
+      </c>
+      <c r="F51">
+        <v>0.75</v>
+      </c>
+      <c r="G51">
+        <v>13.8</v>
+      </c>
+      <c r="H51">
+        <v>-1.55</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K51" t="s">
+        <v>83</v>
+      </c>
+      <c r="L51">
+        <v>21.39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E52">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="F52">
+        <v>0.45</v>
+      </c>
+      <c r="G52">
+        <v>13.7</v>
+      </c>
+      <c r="H52">
+        <v>-2</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L52">
+        <v>27.4</v>
+      </c>
+      <c r="M52" s="7">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E53">
+        <v>7.6</v>
+      </c>
+      <c r="F53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G53">
+        <v>13.8</v>
+      </c>
+      <c r="H53">
+        <v>-1.93</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L53">
+        <v>26.634</v>
+      </c>
+      <c r="M53" s="7">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54">
+        <v>0.2</v>
+      </c>
+      <c r="E54">
+        <v>3.3</v>
+      </c>
+      <c r="F54">
+        <v>0.06</v>
+      </c>
+      <c r="G54">
+        <v>12.7</v>
+      </c>
+      <c r="H54">
+        <v>-0.82</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K54" t="s">
+        <v>28</v>
+      </c>
+      <c r="L54">
+        <v>10.414</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55">
+        <v>2.95</v>
+      </c>
+      <c r="E55">
+        <v>5.32</v>
+      </c>
+      <c r="F55">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G55">
+        <v>11.1</v>
+      </c>
+      <c r="H55">
+        <v>-1.32</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L55">
+        <v>14.651999999999999</v>
+      </c>
+      <c r="M55" s="6">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56">
+        <v>1.68</v>
+      </c>
+      <c r="E56">
+        <v>7.82</v>
+      </c>
+      <c r="F56">
+        <v>0.21</v>
+      </c>
+      <c r="G56">
+        <v>10.9</v>
+      </c>
+      <c r="H56">
+        <v>-1.21</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K56" t="s">
+        <v>36</v>
+      </c>
+      <c r="L56">
+        <v>13.189</v>
+      </c>
+      <c r="M56" s="6">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57">
+        <v>5.13</v>
+      </c>
+      <c r="E57">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>13.6</v>
+      </c>
+      <c r="H57">
+        <v>-2.33</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K57" t="s">
+        <v>104</v>
+      </c>
+      <c r="L57">
+        <v>31.687999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D58">
+        <v>5.75</v>
+      </c>
+      <c r="E58">
+        <v>6.03</v>
+      </c>
+      <c r="F58">
+        <v>0.95</v>
+      </c>
+      <c r="G58">
+        <v>11.8</v>
+      </c>
+      <c r="H58">
+        <v>-1.31</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K58" t="s">
+        <v>52</v>
+      </c>
+      <c r="L58">
+        <v>15.458</v>
+      </c>
+      <c r="M58" s="6">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" t="s">
+        <v>107</v>
+      </c>
+      <c r="D59">
+        <v>1.45</v>
+      </c>
+      <c r="E59">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F59">
+        <v>0.35</v>
+      </c>
+      <c r="G59">
+        <v>14.6</v>
+      </c>
+      <c r="H59">
+        <v>-2.33</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L59">
+        <v>34.018000000000001</v>
+      </c>
+      <c r="M59" s="7">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E60">
+        <v>16</v>
+      </c>
+      <c r="F60">
+        <v>2.4E-2</v>
+      </c>
+      <c r="G60">
+        <v>8.6</v>
+      </c>
+      <c r="H60">
+        <v>-0.81</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L60">
+        <v>6.9660000000000002</v>
+      </c>
+      <c r="M60" s="6">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61">
+        <v>0.68</v>
+      </c>
+      <c r="E61">
+        <v>11</v>
+      </c>
+      <c r="F61">
+        <v>0.06</v>
+      </c>
+      <c r="G61">
+        <v>12</v>
+      </c>
+      <c r="H61">
+        <v>-1.5</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K61" t="s">
+        <v>67</v>
+      </c>
+      <c r="L61">
+        <v>18</v>
+      </c>
+      <c r="M61" s="6">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62">
+        <v>0.39</v>
+      </c>
+      <c r="E62">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F62">
+        <v>0.04</v>
+      </c>
+      <c r="G62">
+        <v>7.4</v>
+      </c>
+      <c r="H62">
+        <v>-0.12</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K62" t="s">
+        <v>11</v>
+      </c>
+      <c r="L62">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="M62" s="6">
+        <v>15.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M62">
+    <sortCondition ref="B2:B62"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>